<commit_message>
Swapped the columns and rows of the dataframe in order to better represent data
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -25,10 +25,10 @@
     <t>Date</t>
   </si>
   <si>
-    <t>Is 1.6 gameplay really better than CS:GO?</t>
+    <t>Brushed DC Motors and How to Drive Them</t>
   </si>
   <si>
-    <t>26 Nov 2021</t>
+    <t>25 Jan 2019</t>
   </si>
 </sst>
 </file>
@@ -386,38 +386,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2">
-      <c r="B1" s="1">
+    <row r="1" spans="1:4">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="2" spans="1:2">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:4">
+      <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3">
-        <v>348577</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="C2">
+        <v>3227096</v>
+      </c>
+      <c r="D2" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Managed to remove the index, the "0" in front of the first row for better representation.
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -16,19 +16,19 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
-    <t>VideoName</t>
-  </si>
-  <si>
     <t>Views</t>
   </si>
   <si>
     <t>Date</t>
   </si>
   <si>
-    <t>Brushed DC Motors and How to Drive Them</t>
+    <t>VideoName</t>
   </si>
   <si>
-    <t>25 Jan 2019</t>
+    <t>A Single Math Equation Makes This Possible</t>
+  </si>
+  <si>
+    <t>11 Mar 2022</t>
   </si>
 </sst>
 </file>
@@ -386,34 +386,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:3">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
     </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="1">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
+    <row r="2" spans="1:3">
+      <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C2">
-        <v>3227099</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="B2">
+        <v>188378</v>
+      </c>
+      <c r="C2" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
I fixed some bugs and made sure the code works with different videos.
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -25,10 +25,10 @@
     <t>VideoName</t>
   </si>
   <si>
-    <t>A Single Math Equation Makes This Possible</t>
+    <t>Bri4ka Honda Legend - Легендата!</t>
   </si>
   <si>
-    <t>11 Mar 2022</t>
+    <t>14 Nov 2017</t>
   </si>
 </sst>
 </file>
@@ -408,7 +408,7 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>188378</v>
+        <v>178443</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>

</xml_diff>